<commit_message>
Test data types are correctly converted
Add data types test file
Implement IDisposable pattern in Importers
</commit_message>
<xml_diff>
--- a/src/GiveCRM.ImportExport/GiveCRM.ImportExport.Test/TestData/MemberData.xlsx
+++ b/src/GiveCRM.ImportExport/GiveCRM.ImportExport.Test/TestData/MemberData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Jill</t>
   </si>
   <si>
-    <t>grant</t>
-  </si>
-  <si>
     <t>W7 5EW</t>
   </si>
   <si>
@@ -175,6 +172,48 @@
   </si>
   <si>
     <t>07757123987</t>
+  </si>
+  <si>
+    <t>Grant</t>
+  </si>
+  <si>
+    <t>jill@give.com</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>john@give.com</t>
+  </si>
+  <si>
+    <t>W1 3QP</t>
+  </si>
+  <si>
+    <t>Miss</t>
+  </si>
+  <si>
+    <t>Cathy</t>
+  </si>
+  <si>
+    <t>Holmes</t>
+  </si>
+  <si>
+    <t>cathy@give.com</t>
+  </si>
+  <si>
+    <t>W1 4QP</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>Monroe</t>
+  </si>
+  <si>
+    <t>brian@give.com</t>
+  </si>
+  <si>
+    <t>W1 5QP</t>
   </si>
 </sst>
 </file>
@@ -517,7 +556,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="B2" sqref="B2:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,10 +678,10 @@
         <v>28</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="P2" t="s">
         <v>29</v>
@@ -668,13 +707,13 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
@@ -686,19 +725,19 @@
         <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L3" t="s">
         <v>27</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P3" t="s">
         <v>30</v>
@@ -721,16 +760,16 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
@@ -742,19 +781,19 @@
         <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="L4" t="s">
         <v>27</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P4" t="s">
         <v>29</v>
@@ -774,19 +813,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
         <v>33</v>
@@ -798,19 +837,19 @@
         <v>25</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="L5" t="s">
         <v>27</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P5" t="s">
         <v>30</v>
@@ -833,16 +872,16 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
         <v>34</v>
@@ -854,19 +893,19 @@
         <v>25</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P6" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Read rows and KVP from Xlsx file
Update data in test files
</commit_message>
<xml_diff>
--- a/src/GiveCRM.ImportExport/GiveCRM.ImportExport.Test/TestData/MemberData.xlsx
+++ b/src/GiveCRM.ImportExport/GiveCRM.ImportExport.Test/TestData/MemberData.xlsx
@@ -66,9 +66,6 @@
     <t>ContactByPhone</t>
   </si>
   <si>
-    <t>ByEmail</t>
-  </si>
-  <si>
     <t>ContactBySMS</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>W1 5QP</t>
+  </si>
+  <si>
+    <t>ContactByEmail</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K6"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,13 +631,13 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -645,55 +645,55 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" t="s">
         <v>29</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -701,55 +701,55 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -757,55 +757,55 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
         <v>55</v>
       </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" t="s">
-        <v>56</v>
-      </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" t="s">
         <v>29</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" t="s">
-        <v>29</v>
-      </c>
-      <c r="S4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -813,55 +813,55 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>58</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
         <v>59</v>
       </c>
-      <c r="E5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
         <v>60</v>
       </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" t="s">
-        <v>61</v>
-      </c>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" t="s">
         <v>29</v>
       </c>
-      <c r="R5" t="s">
-        <v>30</v>
-      </c>
       <c r="S5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -869,55 +869,55 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
         <v>62</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
         <v>63</v>
       </c>
-      <c r="E6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" t="s">
         <v>64</v>
       </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" t="s">
-        <v>65</v>
-      </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" t="s">
-        <v>30</v>
-      </c>
       <c r="R6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>